<commit_message>
finished first draft of ms
</commit_message>
<xml_diff>
--- a/output/anova results 3.xlsx
+++ b/output/anova results 3.xlsx
@@ -19,6 +19,7 @@
     <sheet name="table" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="354">
   <si>
     <t>dryRootBiomass</t>
   </si>
@@ -1017,9 +1018,6 @@
     <t>N (I*)</t>
   </si>
   <si>
-    <t>Stomatal conductance ()</t>
-  </si>
-  <si>
     <t>0.41 (0.11)</t>
   </si>
   <si>
@@ -1065,7 +1063,103 @@
     <t>0.35 (0.08)</t>
   </si>
   <si>
-    <t>cr, cw, wr</t>
+    <r>
+      <t>Photosynthetic rate (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, μmol CO2 m⁻² s⁻¹)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Stomatal conductance (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, mmol m⁻² s⁻¹)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Water use efficiency (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A/Gs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Dry root biomass (g)</t>
+  </si>
+  <si>
+    <t>Dry fine root biomass (g)</t>
+  </si>
+  <si>
+    <t>Dry shoot biomass (g)</t>
+  </si>
+  <si>
+    <t>Fine root DMC (%)</t>
+  </si>
+  <si>
+    <t>SLA (cm² g⁻¹)</t>
+  </si>
+  <si>
+    <t>Stem density (cm² g⁻¹)</t>
+  </si>
+  <si>
+    <t>cw, wr, cr</t>
   </si>
 </sst>
 </file>
@@ -6890,15 +6984,15 @@
         <v>47</v>
       </c>
       <c r="S7">
-        <f t="shared" ref="S7:S24" si="0">E7/C7</f>
+        <f>E7/C7</f>
         <v>1.4102096248307769</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:T24" si="1">I7/G7</f>
+        <f>I7/G7</f>
         <v>0.72114305196684569</v>
       </c>
       <c r="U7">
-        <f t="shared" ref="U7:U24" si="2">M7/K7</f>
+        <f>M7/K7</f>
         <v>1.9456032894671296</v>
       </c>
     </row>
@@ -6950,15 +7044,15 @@
         <v>35</v>
       </c>
       <c r="S8">
-        <f t="shared" si="0"/>
+        <f>E8/C8</f>
         <v>1.21888431169685</v>
       </c>
       <c r="T8">
-        <f t="shared" si="1"/>
+        <f>I8/G8</f>
         <v>1.3453477697733678</v>
       </c>
       <c r="U8">
-        <f t="shared" si="2"/>
+        <f>M8/K8</f>
         <v>0.75763223677652047</v>
       </c>
     </row>
@@ -7092,15 +7186,15 @@
         <v>28</v>
       </c>
       <c r="S13">
-        <f t="shared" si="0"/>
+        <f>E13/C13</f>
         <v>1.5059104252060114</v>
       </c>
       <c r="T13">
-        <f t="shared" si="1"/>
+        <f>I13/G13</f>
         <v>1.2591230281803061</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
+        <f>M13/K13</f>
         <v>1.2907216306784703</v>
       </c>
     </row>
@@ -7149,15 +7243,15 @@
         <v>28</v>
       </c>
       <c r="S14">
-        <f t="shared" si="0"/>
+        <f>E14/C14</f>
         <v>1.3188310504851968</v>
       </c>
       <c r="T14">
-        <f t="shared" si="1"/>
+        <f>I14/G14</f>
         <v>0.941981638581328</v>
       </c>
       <c r="U14">
-        <f t="shared" si="2"/>
+        <f>M14/K14</f>
         <v>1.28045187429324</v>
       </c>
     </row>
@@ -7206,15 +7300,15 @@
         <v>48</v>
       </c>
       <c r="S15">
-        <f t="shared" si="0"/>
+        <f>E15/C15</f>
         <v>1.1265895202184371</v>
       </c>
       <c r="T15">
-        <f t="shared" si="1"/>
+        <f>I15/G15</f>
         <v>1.3640188539453832</v>
       </c>
       <c r="U15">
-        <f t="shared" si="2"/>
+        <f>M15/K15</f>
         <v>1.0011558601135937</v>
       </c>
     </row>
@@ -7383,15 +7477,15 @@
         <v>49</v>
       </c>
       <c r="S22">
-        <f t="shared" si="0"/>
+        <f>E22/C22</f>
         <v>1.5553677314145418</v>
       </c>
       <c r="T22">
-        <f t="shared" si="1"/>
+        <f>I22/G22</f>
         <v>1.1895794546735645</v>
       </c>
       <c r="U22">
-        <f t="shared" si="2"/>
+        <f>M22/K22</f>
         <v>1.172458800210914</v>
       </c>
     </row>
@@ -7443,15 +7537,15 @@
         <v>35</v>
       </c>
       <c r="S23">
-        <f t="shared" si="0"/>
+        <f>E23/C23</f>
         <v>1.1396906183652251</v>
       </c>
       <c r="T23">
-        <f t="shared" si="1"/>
+        <f>I23/G23</f>
         <v>0.88731303695818531</v>
       </c>
       <c r="U23">
-        <f t="shared" si="2"/>
+        <f>M23/K23</f>
         <v>0.92173629223878939</v>
       </c>
     </row>
@@ -7500,15 +7594,15 @@
         <v>28</v>
       </c>
       <c r="S24">
-        <f t="shared" si="0"/>
+        <f>E24/C24</f>
         <v>1.5512543795507434</v>
       </c>
       <c r="T24">
-        <f t="shared" si="1"/>
+        <f>I24/G24</f>
         <v>1.3334840409213848</v>
       </c>
       <c r="U24">
-        <f t="shared" si="2"/>
+        <f>M24/K24</f>
         <v>1.2829650357749656</v>
       </c>
     </row>
@@ -7560,51 +7654,51 @@
         <v>42</v>
       </c>
       <c r="C32" s="24">
-        <f t="shared" ref="C32:N32" si="3">ROUND(C6,2)</f>
+        <f t="shared" ref="C32:N32" si="0">ROUND(C6,2)</f>
         <v>13.41</v>
       </c>
       <c r="D32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>7.58</v>
       </c>
       <c r="E32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>19.25</v>
       </c>
       <c r="F32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>7.47</v>
       </c>
       <c r="G32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>20.9</v>
       </c>
       <c r="H32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>6.83</v>
       </c>
       <c r="I32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>22.06</v>
       </c>
       <c r="J32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>7.68</v>
       </c>
       <c r="K32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>17.149999999999999</v>
       </c>
       <c r="L32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
       <c r="M32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>25.11</v>
       </c>
       <c r="N32" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>6.3</v>
       </c>
     </row>
@@ -7613,51 +7707,51 @@
         <v>44</v>
       </c>
       <c r="C33" s="24">
-        <f t="shared" ref="C33:N33" si="4">ROUND(C7,2)</f>
+        <f t="shared" ref="C33:N33" si="1">ROUND(C7,2)</f>
         <v>13.38</v>
       </c>
       <c r="D33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>3.24</v>
       </c>
       <c r="E33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>18.87</v>
       </c>
       <c r="F33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>8.25</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>11.94</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4.93</v>
       </c>
       <c r="I33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>8.61</v>
       </c>
       <c r="J33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2.13</v>
       </c>
       <c r="K33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>8.6300000000000008</v>
       </c>
       <c r="L33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1.18</v>
       </c>
       <c r="M33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>16.79</v>
       </c>
       <c r="N33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>3.85</v>
       </c>
     </row>
@@ -7666,51 +7760,51 @@
         <v>43</v>
       </c>
       <c r="C34" s="24">
-        <f t="shared" ref="C34:N34" si="5">ROUND(C8,2)</f>
+        <f t="shared" ref="C34:N34" si="2">ROUND(C8,2)</f>
         <v>1</v>
       </c>
       <c r="D34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.43</v>
       </c>
       <c r="E34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1.22</v>
       </c>
       <c r="F34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.62</v>
       </c>
       <c r="G34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1.89</v>
       </c>
       <c r="H34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.53</v>
       </c>
       <c r="I34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.5499999999999998</v>
       </c>
       <c r="J34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.65</v>
       </c>
       <c r="K34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.02</v>
       </c>
       <c r="L34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.35</v>
       </c>
       <c r="M34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1.53</v>
       </c>
       <c r="N34" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.44</v>
       </c>
     </row>
@@ -7780,51 +7874,51 @@
         <v>42</v>
       </c>
       <c r="C39" s="24">
-        <f t="shared" ref="C39:N39" si="6">ROUND(C13,2)</f>
+        <f t="shared" ref="C39:N39" si="3">ROUND(C13,2)</f>
         <v>25.3</v>
       </c>
       <c r="D39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>6.32</v>
       </c>
       <c r="E39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>38.11</v>
       </c>
       <c r="F39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>7.8</v>
       </c>
       <c r="G39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>26.63</v>
       </c>
       <c r="H39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>7.53</v>
       </c>
       <c r="I39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>33.53</v>
       </c>
       <c r="J39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="K39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>27.41</v>
       </c>
       <c r="L39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.81</v>
       </c>
       <c r="M39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>35.380000000000003</v>
       </c>
       <c r="N39" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>7.6</v>
       </c>
     </row>
@@ -7833,51 +7927,51 @@
         <v>44</v>
       </c>
       <c r="C40" s="24">
-        <f t="shared" ref="C40:N40" si="7">ROUND(C14,2)</f>
+        <f t="shared" ref="C40:N40" si="4">ROUND(C14,2)</f>
         <v>17.059999999999999</v>
       </c>
       <c r="D40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4.45</v>
       </c>
       <c r="E40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>22.5</v>
       </c>
       <c r="F40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4.18</v>
       </c>
       <c r="G40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>20.85</v>
       </c>
       <c r="H40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2.37</v>
       </c>
       <c r="I40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>19.64</v>
       </c>
       <c r="J40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2.09</v>
       </c>
       <c r="K40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>16.809999999999999</v>
       </c>
       <c r="L40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2.33</v>
       </c>
       <c r="M40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>21.53</v>
       </c>
       <c r="N40" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>4.8</v>
       </c>
     </row>
@@ -7886,51 +7980,51 @@
         <v>43</v>
       </c>
       <c r="C41" s="24">
-        <f t="shared" ref="C41:N41" si="8">ROUND(C15,2)</f>
+        <f t="shared" ref="C41:N41" si="5">ROUND(C15,2)</f>
         <v>1.5</v>
       </c>
       <c r="D41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
       <c r="E41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.69</v>
       </c>
       <c r="F41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.08</v>
       </c>
       <c r="G41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.26</v>
       </c>
       <c r="H41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.24</v>
       </c>
       <c r="I41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.72</v>
       </c>
       <c r="J41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.23</v>
       </c>
       <c r="K41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.65</v>
       </c>
       <c r="L41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.18</v>
       </c>
       <c r="M41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.65</v>
       </c>
       <c r="N41" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -8030,51 +8124,51 @@
         <v>42</v>
       </c>
       <c r="C48" s="24">
-        <f t="shared" ref="C48:N48" si="9">ROUND(C22,2)</f>
+        <f t="shared" ref="C48:N48" si="6">ROUND(C22,2)</f>
         <v>9.94</v>
       </c>
       <c r="D48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>5.88</v>
       </c>
       <c r="E48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>15.46</v>
       </c>
       <c r="F48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.49</v>
       </c>
       <c r="G48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>15.46</v>
       </c>
       <c r="H48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1.49</v>
       </c>
       <c r="I48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>18.39</v>
       </c>
       <c r="J48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>5.1100000000000003</v>
       </c>
       <c r="K48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>17.989999999999998</v>
       </c>
       <c r="L48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>3.87</v>
       </c>
       <c r="M48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>21.09</v>
       </c>
       <c r="N48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>2.95</v>
       </c>
     </row>
@@ -8083,51 +8177,51 @@
         <v>44</v>
       </c>
       <c r="C49" s="24">
-        <f t="shared" ref="C49:N49" si="10">ROUND(C23,2)</f>
+        <f t="shared" ref="C49:N49" si="7">ROUND(C23,2)</f>
         <v>4.45</v>
       </c>
       <c r="D49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>2.48</v>
       </c>
       <c r="E49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>5.07</v>
       </c>
       <c r="F49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>2.1</v>
       </c>
       <c r="G49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>7.9</v>
       </c>
       <c r="H49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1.42</v>
       </c>
       <c r="I49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>7.01</v>
       </c>
       <c r="J49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1.77</v>
       </c>
       <c r="K49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>9.3000000000000007</v>
       </c>
       <c r="L49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>1.61</v>
       </c>
       <c r="M49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>8.58</v>
       </c>
       <c r="N49" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0.9</v>
       </c>
     </row>
@@ -8136,51 +8230,51 @@
         <v>43</v>
       </c>
       <c r="C50" s="24">
-        <f t="shared" ref="C50:N50" si="11">ROUND(C24,2)</f>
+        <f t="shared" ref="C50:N50" si="8">ROUND(C24,2)</f>
         <v>2.1</v>
       </c>
       <c r="D50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.4</v>
       </c>
       <c r="E50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>3.26</v>
       </c>
       <c r="F50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>1.99</v>
       </c>
       <c r="H50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.25</v>
       </c>
       <c r="I50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>2.65</v>
       </c>
       <c r="J50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.46</v>
       </c>
       <c r="K50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>1.93</v>
       </c>
       <c r="L50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.21</v>
       </c>
       <c r="M50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>2.48</v>
       </c>
       <c r="N50" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.47</v>
       </c>
     </row>
@@ -9671,15 +9765,15 @@
         <v>8.9 (4.17)</v>
       </c>
       <c r="D59" s="24" t="str">
-        <f t="shared" ref="D59" si="3">E34&amp;" "&amp;"("&amp;F34&amp;")"</f>
+        <f>E34&amp;" "&amp;"("&amp;F34&amp;")"</f>
         <v>10.93 (3.67)</v>
       </c>
       <c r="E59" s="24" t="str">
-        <f t="shared" ref="E59" si="4">G34&amp;" "&amp;"("&amp;H34&amp;")"</f>
+        <f>G34&amp;" "&amp;"("&amp;H34&amp;")"</f>
         <v>9.29 (1.65)</v>
       </c>
       <c r="F59" s="24" t="str">
-        <f t="shared" ref="F59" si="5">I34&amp;" "&amp;"("&amp;J34&amp;")"</f>
+        <f>I34&amp;" "&amp;"("&amp;J34&amp;")"</f>
         <v>10.27 (3.13)</v>
       </c>
       <c r="J59" t="s">
@@ -9707,15 +9801,15 @@
         <v>5.64 (2.35)</v>
       </c>
       <c r="D60" s="24" t="str">
-        <f t="shared" ref="D60" si="6">E35&amp;" "&amp;"("&amp;F35&amp;")"</f>
+        <f>E35&amp;" "&amp;"("&amp;F35&amp;")"</f>
         <v>6.02 (2.51)</v>
       </c>
       <c r="E60" s="24" t="str">
-        <f t="shared" ref="E60" si="7">G35&amp;" "&amp;"("&amp;H35&amp;")"</f>
+        <f>G35&amp;" "&amp;"("&amp;H35&amp;")"</f>
         <v>3.74 (0.76)</v>
       </c>
       <c r="F60" s="24" t="str">
-        <f t="shared" ref="F60" si="8">I35&amp;" "&amp;"("&amp;J35&amp;")"</f>
+        <f>I35&amp;" "&amp;"("&amp;J35&amp;")"</f>
         <v>4.64 (0.94)</v>
       </c>
       <c r="J60" t="s">
@@ -9743,15 +9837,15 @@
         <v>2.12 (1.5)</v>
       </c>
       <c r="D61" s="24" t="str">
-        <f t="shared" ref="D61" si="9">E36&amp;" "&amp;"("&amp;F36&amp;")"</f>
+        <f>E36&amp;" "&amp;"("&amp;F36&amp;")"</f>
         <v>2.27 (1.07)</v>
       </c>
       <c r="E61" s="24" t="str">
-        <f t="shared" ref="E61" si="10">G36&amp;" "&amp;"("&amp;H36&amp;")"</f>
+        <f>G36&amp;" "&amp;"("&amp;H36&amp;")"</f>
         <v>1.01 (0.39)</v>
       </c>
       <c r="F61" s="24" t="str">
-        <f t="shared" ref="F61" si="11">I36&amp;" "&amp;"("&amp;J36&amp;")"</f>
+        <f>I36&amp;" "&amp;"("&amp;J36&amp;")"</f>
         <v>1.21 (0.35)</v>
       </c>
       <c r="J61" t="s">
@@ -9818,15 +9912,15 @@
         <v>16.23 (6.8)</v>
       </c>
       <c r="D67" s="24" t="str">
-        <f t="shared" ref="D67" si="12">E42&amp;" "&amp;"("&amp;F42&amp;")"</f>
+        <f>E42&amp;" "&amp;"("&amp;F42&amp;")"</f>
         <v>28.07 (9.21)</v>
       </c>
       <c r="E67" s="24" t="str">
-        <f t="shared" ref="E67" si="13">G42&amp;" "&amp;"("&amp;H42&amp;")"</f>
+        <f>G42&amp;" "&amp;"("&amp;H42&amp;")"</f>
         <v>18.28 (5.26)</v>
       </c>
       <c r="F67" s="24" t="str">
-        <f t="shared" ref="F67" si="14">I42&amp;" "&amp;"("&amp;J42&amp;")"</f>
+        <f>I42&amp;" "&amp;"("&amp;J42&amp;")"</f>
         <v>17.6 (5.59)</v>
       </c>
       <c r="J67" t="s">
@@ -9854,15 +9948,15 @@
         <v>10.44 (3.75)</v>
       </c>
       <c r="D68" s="24" t="str">
-        <f t="shared" ref="D68" si="15">E43&amp;" "&amp;"("&amp;F43&amp;")"</f>
+        <f>E43&amp;" "&amp;"("&amp;F43&amp;")"</f>
         <v>17.19 (5.66)</v>
       </c>
       <c r="E68" s="24" t="str">
-        <f t="shared" ref="E68" si="16">G43&amp;" "&amp;"("&amp;H43&amp;")"</f>
+        <f>G43&amp;" "&amp;"("&amp;H43&amp;")"</f>
         <v>11.97 (3.28)</v>
       </c>
       <c r="F68" s="24" t="str">
-        <f t="shared" ref="F68" si="17">I43&amp;" "&amp;"("&amp;J43&amp;")"</f>
+        <f>I43&amp;" "&amp;"("&amp;J43&amp;")"</f>
         <v>10.55 (3)</v>
       </c>
       <c r="J68" t="s">
@@ -9890,15 +9984,15 @@
         <v>5.79 (3.1)</v>
       </c>
       <c r="D69" s="24" t="str">
-        <f t="shared" ref="D69" si="18">E44&amp;" "&amp;"("&amp;F44&amp;")"</f>
+        <f>E44&amp;" "&amp;"("&amp;F44&amp;")"</f>
         <v>10.88 (3.67)</v>
       </c>
       <c r="E69" s="24" t="str">
-        <f t="shared" ref="E69" si="19">G44&amp;" "&amp;"("&amp;H44&amp;")"</f>
+        <f>G44&amp;" "&amp;"("&amp;H44&amp;")"</f>
         <v>6.31 (2.07)</v>
       </c>
       <c r="F69" s="24" t="str">
-        <f t="shared" ref="F69" si="20">I44&amp;" "&amp;"("&amp;J44&amp;")"</f>
+        <f>I44&amp;" "&amp;"("&amp;J44&amp;")"</f>
         <v>7.05 (2.75)</v>
       </c>
       <c r="J69" t="s">
@@ -9926,15 +10020,15 @@
         <v>1.66 (1.23)</v>
       </c>
       <c r="D70" s="24" t="str">
-        <f t="shared" ref="D70" si="21">E45&amp;" "&amp;"("&amp;F45&amp;")"</f>
+        <f>E45&amp;" "&amp;"("&amp;F45&amp;")"</f>
         <v>4.11 (1.96)</v>
       </c>
       <c r="E70" s="24" t="str">
-        <f t="shared" ref="E70" si="22">G45&amp;" "&amp;"("&amp;H45&amp;")"</f>
+        <f>G45&amp;" "&amp;"("&amp;H45&amp;")"</f>
         <v>1.95 (0.73)</v>
       </c>
       <c r="F70" s="24" t="str">
-        <f t="shared" ref="F70" si="23">I45&amp;" "&amp;"("&amp;J45&amp;")"</f>
+        <f>I45&amp;" "&amp;"("&amp;J45&amp;")"</f>
         <v>2.61 (1.31)</v>
       </c>
       <c r="J70" t="s">
@@ -10001,15 +10095,15 @@
         <v>37.78 (7.83)</v>
       </c>
       <c r="D76" s="24" t="str">
-        <f t="shared" ref="D76" si="24">E51&amp;" "&amp;"("&amp;F51&amp;")"</f>
+        <f>E51&amp;" "&amp;"("&amp;F51&amp;")"</f>
         <v>36.95 (8.09)</v>
       </c>
       <c r="E76" s="24" t="str">
-        <f t="shared" ref="E76" si="25">G51&amp;" "&amp;"("&amp;H51&amp;")"</f>
+        <f>G51&amp;" "&amp;"("&amp;H51&amp;")"</f>
         <v>40.58 (15.14)</v>
       </c>
       <c r="F76" s="24" t="str">
-        <f t="shared" ref="F76" si="26">I51&amp;" "&amp;"("&amp;J51&amp;")"</f>
+        <f>I51&amp;" "&amp;"("&amp;J51&amp;")"</f>
         <v>36.66 (14.46)</v>
       </c>
       <c r="J76" t="s">
@@ -10037,15 +10131,15 @@
         <v>22.93 (5.31)</v>
       </c>
       <c r="D77" s="24" t="str">
-        <f t="shared" ref="D77" si="27">E52&amp;" "&amp;"("&amp;F52&amp;")"</f>
+        <f>E52&amp;" "&amp;"("&amp;F52&amp;")"</f>
         <v>22.63 (6.13)</v>
       </c>
       <c r="E77" s="24" t="str">
-        <f t="shared" ref="E77" si="28">G52&amp;" "&amp;"("&amp;H52&amp;")"</f>
+        <f>G52&amp;" "&amp;"("&amp;H52&amp;")"</f>
         <v>26.49 (10.35)</v>
       </c>
       <c r="F77" s="24" t="str">
-        <f t="shared" ref="F77" si="29">I52&amp;" "&amp;"("&amp;J52&amp;")"</f>
+        <f>I52&amp;" "&amp;"("&amp;J52&amp;")"</f>
         <v>23.23 (8.49)</v>
       </c>
       <c r="J77" t="s">
@@ -10073,15 +10167,15 @@
         <v>14.85 (3.5)</v>
       </c>
       <c r="D78" s="24" t="str">
-        <f t="shared" ref="D78" si="30">E53&amp;" "&amp;"("&amp;F53&amp;")"</f>
+        <f>E53&amp;" "&amp;"("&amp;F53&amp;")"</f>
         <v>14.32 (2.58)</v>
       </c>
       <c r="E78" s="24" t="str">
-        <f t="shared" ref="E78" si="31">G53&amp;" "&amp;"("&amp;H53&amp;")"</f>
+        <f>G53&amp;" "&amp;"("&amp;H53&amp;")"</f>
         <v>14.09 (5.73)</v>
       </c>
       <c r="F78" s="24" t="str">
-        <f t="shared" ref="F78:F79" si="32">I53&amp;" "&amp;"("&amp;J53&amp;")"</f>
+        <f>I53&amp;" "&amp;"("&amp;J53&amp;")"</f>
         <v>13.42 (6.51)</v>
       </c>
       <c r="J78" t="s">
@@ -10109,15 +10203,15 @@
         <v>2.64 (1.84)</v>
       </c>
       <c r="D79" s="24" t="str">
-        <f t="shared" ref="D79" si="33">E54&amp;" "&amp;"("&amp;F54&amp;")"</f>
+        <f>E54&amp;" "&amp;"("&amp;F54&amp;")"</f>
         <v>1.73 (0.93)</v>
       </c>
       <c r="E79" s="24" t="str">
-        <f t="shared" ref="E79" si="34">G54&amp;" "&amp;"("&amp;H54&amp;")"</f>
+        <f>G54&amp;" "&amp;"("&amp;H54&amp;")"</f>
         <v>3.69 (2.73)</v>
       </c>
       <c r="F79" s="24" t="str">
-        <f t="shared" si="32"/>
+        <f>I54&amp;" "&amp;"("&amp;J54&amp;")"</f>
         <v>3.82 (2.22)</v>
       </c>
       <c r="J79" t="s">
@@ -10153,13 +10247,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A46" sqref="A33:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -10238,7 +10332,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>212</v>
@@ -10265,25 +10359,25 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
+        <v>345</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>332</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>333</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>134</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>26</v>
@@ -10292,7 +10386,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>224</v>
@@ -10332,7 +10426,7 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>273</v>
@@ -10397,7 +10491,7 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>277</v>
@@ -10463,7 +10557,7 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
-        <v>319</v>
+        <v>349</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>269</v>
@@ -10555,7 +10649,9 @@
       <c r="H12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="36"/>
@@ -10570,7 +10666,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>61</v>
@@ -10599,7 +10695,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>85</v>
@@ -10628,7 +10724,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>97</v>
@@ -10690,7 +10786,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>230</v>
@@ -10717,25 +10813,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="D21" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="F21" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>338</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>339</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>26</v>
@@ -10744,7 +10840,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>242</v>
@@ -10782,7 +10878,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>289</v>
@@ -10805,7 +10901,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>293</v>
@@ -10828,7 +10924,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
-        <v>319</v>
+        <v>349</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>285</v>
@@ -10889,7 +10985,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>118</v>
@@ -10916,7 +11012,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>139</v>
@@ -10943,7 +11039,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>151</v>
@@ -10980,7 +11076,7 @@
       <c r="I32" s="32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="37" t="s">
         <v>211</v>
       </c>
       <c r="B33" s="11"/>
@@ -11005,7 +11101,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>248</v>
@@ -11034,36 +11130,36 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="B36" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>340</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>341</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>115</v>
       </c>
       <c r="E36" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="G36" s="10" t="s">
         <v>343</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>344</v>
       </c>
       <c r="H36" s="11" t="s">
         <v>27</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>259</v>
@@ -11101,7 +11197,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="36" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>305</v>
@@ -11124,7 +11220,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>309</v>
@@ -11147,7 +11243,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
-        <v>319</v>
+        <v>349</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>301</v>
@@ -11208,7 +11304,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="36" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>173</v>
@@ -11237,7 +11333,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="36" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>189</v>
@@ -11266,7 +11362,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
-        <v>326</v>
+        <v>352</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>201</v>
@@ -11289,9 +11385,7 @@
       <c r="H46" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="32" t="s">
-        <v>38</v>
-      </c>
+      <c r="I46" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>